<commit_message>
1) correções do registers;
</commit_message>
<xml_diff>
--- a/CoParticipacaoWebService/src/test/resources/cargill/input/CARGILL.ISENTO.201811.003.xlsx
+++ b/CoParticipacaoWebService/src/test/resources/cargill/input/CARGILL.ISENTO.201811.003.xlsx
@@ -185,7 +185,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -211,12 +211,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -236,9 +236,9 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="10.71"/>
@@ -350,7 +350,12 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="str">
+        <f aca="false">IF(C5="",LEFT(RIGHT(SUBSTITUTE(TRIM(B5)," ",),16),15),LEFT(RIGHT(SUBSTITUTE(TRIM(C5)," ",),16),15))</f>
+        <v/>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="str">
         <f aca="false">IF(C6="",LEFT(RIGHT(SUBSTITUTE(TRIM(B6)," ",),16),15),LEFT(RIGHT(SUBSTITUTE(TRIM(C6)," ",),16),15))</f>

</xml_diff>